<commit_message>
rename Data_processing.py to Data_processor.py
remove redundant import in Data_processor.py
</commit_message>
<xml_diff>
--- a/AQI_report_2022-04-18.xlsx
+++ b/AQI_report_2022-04-18.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="66">
   <si>
     <t>臺北市</t>
   </si>
@@ -1466,13 +1466,13 @@
         <v>9</v>
       </c>
       <c r="D4" s="2">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0</v>
+        <v>87</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="2" customFormat="1" ht="35" customHeight="1">
@@ -1680,10 +1680,10 @@
         <v>1</v>
       </c>
       <c r="D15" s="2">
-        <v>30.31</v>
+        <v>32.92</v>
       </c>
       <c r="E15" s="2">
-        <v>81.23</v>
+        <v>87.92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>